<commit_message>
sheets version updated field renamed
</commit_message>
<xml_diff>
--- a/AvantisChannelList.xlsx
+++ b/AvantisChannelList.xlsx
@@ -50,7 +50,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="424">
   <si>
-    <t xml:space="preserve">Process?</t>
+    <t xml:space="preserve">Enabled</t>
   </si>
   <si>
     <t xml:space="preserve">Channel</t>
@@ -26271,7 +26271,7 @@
         <v>422</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>423</v>

</xml_diff>